<commit_message>
* add looging * fix typos and bugs * update config * update samplesheet
</commit_message>
<xml_diff>
--- a/sample_sheet.xlsx
+++ b/sample_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiaraparrillo/Desktop/Progetti/ALOA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E7F214-0A93-0342-BF85-9050DC7D7049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6905019C-1F44-7747-B391-0330CDF177FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17200" yWindow="500" windowWidth="19520" windowHeight="18300" xr2:uid="{6450AEE9-C1E0-473E-8F39-509818AF7DA8}"/>
+    <workbookView xWindow="5240" yWindow="2300" windowWidth="19520" windowHeight="18300" xr2:uid="{6450AEE9-C1E0-473E-8F39-509818AF7DA8}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Group</t>
   </si>
@@ -47,25 +47,28 @@
     <t>sbj_ID</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
+    <t>Set4_1-6plex_S</t>
+  </si>
+  <si>
+    <t>Set4_1-6plex_T</t>
+  </si>
+  <si>
+    <t>Set8_11-6plex_S</t>
+  </si>
+  <si>
+    <t>Set8_11-6plex_T</t>
+  </si>
+  <si>
+    <t>Set12_20-6plex_S</t>
+  </si>
+  <si>
+    <t>Set12_20-6plex_T</t>
+  </si>
+  <si>
+    <t>Stroma</t>
+  </si>
+  <si>
+    <t>Tumor</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -463,7 +466,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -471,7 +474,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -479,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -487,17 +490,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>